<commit_message>
Minor correction of assignation of values
</commit_message>
<xml_diff>
--- a/stockData.xlsx
+++ b/stockData.xlsx
@@ -422,7 +422,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -431,14 +431,19 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>02-07-2023</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>02-07-2023</t>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>05-07-2023</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>05-07-2023</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>05-07-2023</t>
         </is>
       </c>
     </row>
@@ -448,31 +453,53 @@
           <t>1er Janvier</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>+15.31%</t>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>+14.13%</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
         <v>11.87</v>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="2" t="n">
+        <v>9.289999999999999</v>
+      </c>
+      <c r="E2" s="2" t="n"/>
+      <c r="F2" s="2" t="n"/>
+      <c r="G2" s="2" t="n"/>
+      <c r="H2" s="2" t="n"/>
+      <c r="I2" s="2" t="inlineStr">
         <is>
           <t>1er Janvier</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>+15.31%</t>
-        </is>
-      </c>
-      <c r="F2" s="2" t="n">
-        <v>11.87</v>
-      </c>
-      <c r="G2" s="2" t="n">
+      <c r="J2" s="2" t="inlineStr">
+        <is>
+          <t>+14.13%</t>
+        </is>
+      </c>
+      <c r="K2" s="2" t="n">
+        <v>11.87</v>
+      </c>
+      <c r="L2" s="2" t="n">
         <v>9.289999999999999</v>
       </c>
-      <c r="H2" s="2" t="n"/>
+      <c r="M2" s="2" t="inlineStr">
+        <is>
+          <t>1er Janvier</t>
+        </is>
+      </c>
+      <c r="N2" s="2" t="inlineStr">
+        <is>
+          <t>+14.13%</t>
+        </is>
+      </c>
+      <c r="O2" t="n">
+        <v>11.87</v>
+      </c>
+      <c r="P2" t="n">
+        <v>9.289999999999999</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -482,27 +509,46 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>+3.10%</t>
+          <t>-1.51%</t>
         </is>
       </c>
       <c r="C3" t="n">
         <v>10.81</v>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" t="n">
+        <v>10.51</v>
+      </c>
+      <c r="I3" t="inlineStr">
         <is>
           <t>1 semaine</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>+3.10%</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>-1.51%</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
         <v>10.81</v>
       </c>
-      <c r="G3" t="n">
-        <v>10.28</v>
+      <c r="L3" t="n">
+        <v>10.51</v>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>1 semaine</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>-1.51%</t>
+        </is>
+      </c>
+      <c r="O3" t="n">
+        <v>10.81</v>
+      </c>
+      <c r="P3" t="n">
+        <v>10.51</v>
       </c>
     </row>
     <row r="4">
@@ -513,26 +559,45 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>-4.21%</t>
+          <t>-0.88%</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>11.3</v>
-      </c>
-      <c r="D4" t="inlineStr">
+        <v>10.81</v>
+      </c>
+      <c r="D4" t="n">
+        <v>10.21</v>
+      </c>
+      <c r="I4" t="inlineStr">
         <is>
           <t>1 mois</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>-4.21%</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>11.3</v>
-      </c>
-      <c r="G4" t="n">
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>-0.88%</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
+        <v>10.81</v>
+      </c>
+      <c r="L4" t="n">
+        <v>10.21</v>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>1 mois</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>-0.88%</t>
+        </is>
+      </c>
+      <c r="O4" t="n">
+        <v>10.81</v>
+      </c>
+      <c r="P4" t="n">
         <v>10.21</v>
       </c>
     </row>
@@ -544,26 +609,45 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>-2.28%</t>
+          <t>-7.57%</t>
         </is>
       </c>
       <c r="C5" t="n">
         <v>11.87</v>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D5" t="n">
+        <v>10.21</v>
+      </c>
+      <c r="I5" t="inlineStr">
         <is>
           <t>3 mois</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>-2.28%</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>11.87</v>
-      </c>
-      <c r="G5" t="n">
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>-7.57%</t>
+        </is>
+      </c>
+      <c r="K5" t="n">
+        <v>11.87</v>
+      </c>
+      <c r="L5" t="n">
+        <v>10.21</v>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>3 mois</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>-7.57%</t>
+        </is>
+      </c>
+      <c r="O5" t="n">
+        <v>11.87</v>
+      </c>
+      <c r="P5" t="n">
         <v>10.21</v>
       </c>
     </row>
@@ -575,27 +659,46 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>+13.92%</t>
+          <t>+7.09%</t>
         </is>
       </c>
       <c r="C6" t="n">
         <v>11.87</v>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="D6" t="n">
+        <v>9.49</v>
+      </c>
+      <c r="I6" t="inlineStr">
         <is>
           <t>6 mois</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>+13.92%</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>11.87</v>
-      </c>
-      <c r="G6" t="n">
-        <v>9.289999999999999</v>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>+7.09%</t>
+        </is>
+      </c>
+      <c r="K6" t="n">
+        <v>11.87</v>
+      </c>
+      <c r="L6" t="n">
+        <v>9.49</v>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>6 mois</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>+7.09%</t>
+        </is>
+      </c>
+      <c r="O6" t="n">
+        <v>11.87</v>
+      </c>
+      <c r="P6" t="n">
+        <v>9.49</v>
       </c>
     </row>
     <row r="7">
@@ -606,26 +709,45 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>-5.12%</t>
+          <t>-3.83%</t>
         </is>
       </c>
       <c r="C7" t="n">
         <v>11.87</v>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D7" t="n">
+        <v>9.08</v>
+      </c>
+      <c r="I7" t="inlineStr">
         <is>
           <t>1 an</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>-5.12%</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>11.87</v>
-      </c>
-      <c r="G7" t="n">
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>-3.83%</t>
+        </is>
+      </c>
+      <c r="K7" t="n">
+        <v>11.87</v>
+      </c>
+      <c r="L7" t="n">
+        <v>9.08</v>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>1 an</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>-3.83%</t>
+        </is>
+      </c>
+      <c r="O7" t="n">
+        <v>11.87</v>
+      </c>
+      <c r="P7" t="n">
         <v>9.08</v>
       </c>
     </row>
@@ -637,26 +759,45 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>+0.96%</t>
+          <t>-3.27%</t>
         </is>
       </c>
       <c r="C8" t="n">
         <v>11.94</v>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D8" t="n">
+        <v>8.630000000000001</v>
+      </c>
+      <c r="I8" t="inlineStr">
         <is>
           <t>3 ans</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>+0.96%</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>-3.27%</t>
+        </is>
+      </c>
+      <c r="K8" t="n">
         <v>11.94</v>
       </c>
-      <c r="G8" t="n">
+      <c r="L8" t="n">
+        <v>8.630000000000001</v>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>3 ans</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>-3.27%</t>
+        </is>
+      </c>
+      <c r="O8" t="n">
+        <v>11.94</v>
+      </c>
+      <c r="P8" t="n">
         <v>8.630000000000001</v>
       </c>
     </row>
@@ -668,26 +809,45 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>-24.87%</t>
+          <t>-28.72%</t>
         </is>
       </c>
       <c r="C9" t="n">
         <v>15.38</v>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D9" t="n">
+        <v>8.630000000000001</v>
+      </c>
+      <c r="I9" t="inlineStr">
         <is>
           <t>5 ans</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>-24.87%</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>-28.72%</t>
+        </is>
+      </c>
+      <c r="K9" t="n">
         <v>15.38</v>
       </c>
-      <c r="G9" t="n">
+      <c r="L9" t="n">
+        <v>8.630000000000001</v>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>5 ans</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>-28.72%</t>
+        </is>
+      </c>
+      <c r="O9" t="n">
+        <v>15.38</v>
+      </c>
+      <c r="P9" t="n">
         <v>8.630000000000001</v>
       </c>
     </row>
@@ -699,27 +859,46 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>+47.61%</t>
+          <t>+46.81%</t>
         </is>
       </c>
       <c r="C10" t="n">
         <v>16.98</v>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="D10" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="I10" t="inlineStr">
         <is>
           <t>10 ans</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>+47.61%</t>
-        </is>
-      </c>
-      <c r="F10" t="n">
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>+46.81%</t>
+        </is>
+      </c>
+      <c r="K10" t="n">
         <v>16.98</v>
       </c>
-      <c r="G10" t="n">
-        <v>7.03</v>
+      <c r="L10" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>10 ans</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>+46.81%</t>
+        </is>
+      </c>
+      <c r="O10" t="n">
+        <v>16.98</v>
+      </c>
+      <c r="P10" t="n">
+        <v>7.1</v>
       </c>
     </row>
     <row r="11">
@@ -728,18 +907,29 @@
           <t>MM20</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="D11" t="n">
+        <v>10.46</v>
+      </c>
+      <c r="I11" t="inlineStr">
         <is>
           <t>MM20</t>
         </is>
       </c>
-      <c r="E11" t="n">
+      <c r="L11" t="n">
+        <v>10.46</v>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>MM20</t>
+        </is>
+      </c>
+      <c r="N11" t="n">
         <v/>
       </c>
-      <c r="F11" t="n">
+      <c r="O11" t="n">
         <v/>
       </c>
-      <c r="G11" t="n">
+      <c r="P11" t="n">
         <v>10.46</v>
       </c>
     </row>
@@ -749,19 +939,30 @@
           <t>MM50</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D12" t="n">
+        <v>11.02</v>
+      </c>
+      <c r="I12" t="inlineStr">
         <is>
           <t>MM50</t>
         </is>
       </c>
-      <c r="E12" t="n">
+      <c r="L12" t="n">
+        <v>11.02</v>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>MM50</t>
+        </is>
+      </c>
+      <c r="N12" t="n">
         <v/>
       </c>
-      <c r="F12" t="n">
+      <c r="O12" t="n">
         <v/>
       </c>
-      <c r="G12" t="n">
-        <v>11.07</v>
+      <c r="P12" t="n">
+        <v>11.02</v>
       </c>
     </row>
     <row r="13">
@@ -770,19 +971,30 @@
           <t>MM100</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D13" t="n">
+        <v>10.98</v>
+      </c>
+      <c r="I13" t="inlineStr">
         <is>
           <t>MM100</t>
         </is>
       </c>
-      <c r="E13" t="n">
+      <c r="L13" t="n">
+        <v>10.98</v>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>MM100</t>
+        </is>
+      </c>
+      <c r="N13" t="n">
         <v/>
       </c>
-      <c r="F13" t="n">
+      <c r="O13" t="n">
         <v/>
       </c>
-      <c r="G13" t="n">
-        <v>10.95</v>
+      <c r="P13" t="n">
+        <v>10.98</v>
       </c>
     </row>
     <row r="14">
@@ -791,26 +1003,38 @@
           <t>RSI14</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="D14" t="n">
+        <v>65.53</v>
+      </c>
+      <c r="I14" t="inlineStr">
         <is>
           <t>RSI14</t>
         </is>
       </c>
-      <c r="E14" t="n">
+      <c r="L14" t="n">
+        <v>65.53</v>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>RSI14</t>
+        </is>
+      </c>
+      <c r="N14" t="n">
         <v/>
       </c>
-      <c r="F14" t="n">
+      <c r="O14" t="n">
         <v/>
       </c>
-      <c r="G14" t="n">
-        <v>56.6</v>
+      <c r="P14" t="n">
+        <v>65.53</v>
       </c>
     </row>
     <row r="15"/>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:H1"/>
+  <mergeCells count="3">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Improve shifting of data after first day
</commit_message>
<xml_diff>
--- a/stockData.xlsx
+++ b/stockData.xlsx
@@ -422,7 +422,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,11 +441,6 @@
           <t>05-07-2023</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>05-07-2023</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -464,42 +459,23 @@
       <c r="D2" s="2" t="n">
         <v>9.289999999999999</v>
       </c>
-      <c r="E2" s="2" t="n"/>
-      <c r="F2" s="2" t="n"/>
-      <c r="G2" s="2" t="n"/>
-      <c r="H2" s="2" t="n"/>
-      <c r="I2" s="2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>1er Janvier</t>
         </is>
       </c>
-      <c r="J2" s="2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>+14.13%</t>
         </is>
       </c>
-      <c r="K2" s="2" t="n">
+      <c r="G2" s="2" t="n">
         <v>11.87</v>
       </c>
-      <c r="L2" s="2" t="n">
+      <c r="H2" s="2" t="n">
         <v>9.289999999999999</v>
       </c>
-      <c r="M2" s="2" t="inlineStr">
-        <is>
-          <t>1er Janvier</t>
-        </is>
-      </c>
-      <c r="N2" s="2" t="inlineStr">
-        <is>
-          <t>+14.13%</t>
-        </is>
-      </c>
-      <c r="O2" t="n">
-        <v>11.87</v>
-      </c>
-      <c r="P2" t="n">
-        <v>9.289999999999999</v>
-      </c>
+      <c r="I2" s="2" t="n"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -518,36 +494,20 @@
       <c r="D3" t="n">
         <v>10.51</v>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>1 semaine</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>-1.51%</t>
         </is>
       </c>
-      <c r="K3" t="n">
+      <c r="G3" t="n">
         <v>10.81</v>
       </c>
-      <c r="L3" t="n">
-        <v>10.51</v>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>1 semaine</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>-1.51%</t>
-        </is>
-      </c>
-      <c r="O3" t="n">
-        <v>10.81</v>
-      </c>
-      <c r="P3" t="n">
+      <c r="H3" t="n">
         <v>10.51</v>
       </c>
     </row>
@@ -568,36 +528,20 @@
       <c r="D4" t="n">
         <v>10.21</v>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>1 mois</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>-0.88%</t>
         </is>
       </c>
-      <c r="K4" t="n">
+      <c r="G4" t="n">
         <v>10.81</v>
       </c>
-      <c r="L4" t="n">
-        <v>10.21</v>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>1 mois</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>-0.88%</t>
-        </is>
-      </c>
-      <c r="O4" t="n">
-        <v>10.81</v>
-      </c>
-      <c r="P4" t="n">
+      <c r="H4" t="n">
         <v>10.21</v>
       </c>
     </row>
@@ -618,36 +562,20 @@
       <c r="D5" t="n">
         <v>10.21</v>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>3 mois</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>-7.57%</t>
         </is>
       </c>
-      <c r="K5" t="n">
+      <c r="G5" t="n">
         <v>11.87</v>
       </c>
-      <c r="L5" t="n">
-        <v>10.21</v>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>3 mois</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>-7.57%</t>
-        </is>
-      </c>
-      <c r="O5" t="n">
-        <v>11.87</v>
-      </c>
-      <c r="P5" t="n">
+      <c r="H5" t="n">
         <v>10.21</v>
       </c>
     </row>
@@ -668,36 +596,20 @@
       <c r="D6" t="n">
         <v>9.49</v>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>6 mois</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>+7.09%</t>
         </is>
       </c>
-      <c r="K6" t="n">
+      <c r="G6" t="n">
         <v>11.87</v>
       </c>
-      <c r="L6" t="n">
-        <v>9.49</v>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>6 mois</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>+7.09%</t>
-        </is>
-      </c>
-      <c r="O6" t="n">
-        <v>11.87</v>
-      </c>
-      <c r="P6" t="n">
+      <c r="H6" t="n">
         <v>9.49</v>
       </c>
     </row>
@@ -718,36 +630,20 @@
       <c r="D7" t="n">
         <v>9.08</v>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>1 an</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>-3.83%</t>
         </is>
       </c>
-      <c r="K7" t="n">
+      <c r="G7" t="n">
         <v>11.87</v>
       </c>
-      <c r="L7" t="n">
-        <v>9.08</v>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>1 an</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>-3.83%</t>
-        </is>
-      </c>
-      <c r="O7" t="n">
-        <v>11.87</v>
-      </c>
-      <c r="P7" t="n">
+      <c r="H7" t="n">
         <v>9.08</v>
       </c>
     </row>
@@ -768,36 +664,20 @@
       <c r="D8" t="n">
         <v>8.630000000000001</v>
       </c>
-      <c r="I8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>3 ans</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>-3.27%</t>
         </is>
       </c>
-      <c r="K8" t="n">
+      <c r="G8" t="n">
         <v>11.94</v>
       </c>
-      <c r="L8" t="n">
-        <v>8.630000000000001</v>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>3 ans</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>-3.27%</t>
-        </is>
-      </c>
-      <c r="O8" t="n">
-        <v>11.94</v>
-      </c>
-      <c r="P8" t="n">
+      <c r="H8" t="n">
         <v>8.630000000000001</v>
       </c>
     </row>
@@ -818,36 +698,20 @@
       <c r="D9" t="n">
         <v>8.630000000000001</v>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>5 ans</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>-28.72%</t>
         </is>
       </c>
-      <c r="K9" t="n">
+      <c r="G9" t="n">
         <v>15.38</v>
       </c>
-      <c r="L9" t="n">
-        <v>8.630000000000001</v>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>5 ans</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>-28.72%</t>
-        </is>
-      </c>
-      <c r="O9" t="n">
-        <v>15.38</v>
-      </c>
-      <c r="P9" t="n">
+      <c r="H9" t="n">
         <v>8.630000000000001</v>
       </c>
     </row>
@@ -868,36 +732,20 @@
       <c r="D10" t="n">
         <v>7.1</v>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>10 ans</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>+46.81%</t>
         </is>
       </c>
-      <c r="K10" t="n">
+      <c r="G10" t="n">
         <v>16.98</v>
       </c>
-      <c r="L10" t="n">
-        <v>7.1</v>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>10 ans</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>+46.81%</t>
-        </is>
-      </c>
-      <c r="O10" t="n">
-        <v>16.98</v>
-      </c>
-      <c r="P10" t="n">
+      <c r="H10" t="n">
         <v>7.1</v>
       </c>
     </row>
@@ -910,26 +758,18 @@
       <c r="D11" t="n">
         <v>10.46</v>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>MM20</t>
         </is>
       </c>
-      <c r="L11" t="n">
-        <v>10.46</v>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>MM20</t>
-        </is>
-      </c>
-      <c r="N11" t="n">
+      <c r="F11" t="n">
         <v/>
       </c>
-      <c r="O11" t="n">
+      <c r="G11" t="n">
         <v/>
       </c>
-      <c r="P11" t="n">
+      <c r="H11" t="n">
         <v>10.46</v>
       </c>
     </row>
@@ -942,26 +782,18 @@
       <c r="D12" t="n">
         <v>11.02</v>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>MM50</t>
         </is>
       </c>
-      <c r="L12" t="n">
-        <v>11.02</v>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>MM50</t>
-        </is>
-      </c>
-      <c r="N12" t="n">
+      <c r="F12" t="n">
         <v/>
       </c>
-      <c r="O12" t="n">
+      <c r="G12" t="n">
         <v/>
       </c>
-      <c r="P12" t="n">
+      <c r="H12" t="n">
         <v>11.02</v>
       </c>
     </row>
@@ -974,26 +806,18 @@
       <c r="D13" t="n">
         <v>10.98</v>
       </c>
-      <c r="I13" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>MM100</t>
         </is>
       </c>
-      <c r="L13" t="n">
-        <v>10.98</v>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>MM100</t>
-        </is>
-      </c>
-      <c r="N13" t="n">
+      <c r="F13" t="n">
         <v/>
       </c>
-      <c r="O13" t="n">
+      <c r="G13" t="n">
         <v/>
       </c>
-      <c r="P13" t="n">
+      <c r="H13" t="n">
         <v>10.98</v>
       </c>
     </row>
@@ -1006,35 +830,26 @@
       <c r="D14" t="n">
         <v>65.53</v>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>RSI14</t>
         </is>
       </c>
-      <c r="L14" t="n">
-        <v>65.53</v>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>RSI14</t>
-        </is>
-      </c>
-      <c r="N14" t="n">
+      <c r="F14" t="n">
         <v/>
       </c>
-      <c r="O14" t="n">
+      <c r="G14" t="n">
         <v/>
       </c>
-      <c r="P14" t="n">
+      <c r="H14" t="n">
         <v>65.53</v>
       </c>
     </row>
     <row r="15"/>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Improve headers and data alignment
</commit_message>
<xml_diff>
--- a/stockData.xlsx
+++ b/stockData.xlsx
@@ -422,7 +422,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -431,12 +431,12 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>05-07-2023</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>05-07-2023</t>
         </is>
@@ -448,7 +448,7 @@
           <t>1er Janvier</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>+14.13%</t>
         </is>
@@ -464,7 +464,7 @@
           <t>1er Janvier</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" s="2" t="inlineStr">
         <is>
           <t>+14.13%</t>
         </is>
@@ -475,7 +475,6 @@
       <c r="H2" s="2" t="n">
         <v>9.289999999999999</v>
       </c>
-      <c r="I2" s="2" t="n"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -848,8 +847,8 @@
     <row r="15"/>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:H1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add new worksheet (if file already existed) for newly added companies to the list to get the data from.
</commit_message>
<xml_diff>
--- a/stockData.xlsx
+++ b/stockData.xlsx
@@ -437,6 +437,11 @@
           <t>16-07-2023</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>16-07-2023</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -455,7 +460,22 @@
       <c r="D2" s="2" t="n">
         <v>9.289999999999999</v>
       </c>
-      <c r="E2" s="2" t="n"/>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>1er Janvier</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>+13.03%</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>11.87</v>
+      </c>
+      <c r="H2" t="n">
+        <v>9.289999999999999</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -474,6 +494,22 @@
       <c r="D3" t="n">
         <v>10.31</v>
       </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>1 semaine</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>+1.10%</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>10.59</v>
+      </c>
+      <c r="H3" t="n">
+        <v>10.31</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -492,6 +528,22 @@
       <c r="D4" t="n">
         <v>10.18</v>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>1 mois</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>+1.27%</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>10.81</v>
+      </c>
+      <c r="H4" t="n">
+        <v>10.18</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -510,6 +562,22 @@
       <c r="D5" t="n">
         <v>10.18</v>
       </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>3 mois</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>-7.79%</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>11.87</v>
+      </c>
+      <c r="H5" t="n">
+        <v>10.18</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -528,6 +596,22 @@
       <c r="D6" t="n">
         <v>9.49</v>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>6 mois</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>+8.14%</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>11.87</v>
+      </c>
+      <c r="H6" t="n">
+        <v>9.49</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -546,6 +630,22 @@
       <c r="D7" t="n">
         <v>9.08</v>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>1 an</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>-0.59%</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>11.87</v>
+      </c>
+      <c r="H7" t="n">
+        <v>9.08</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -564,6 +664,22 @@
       <c r="D8" t="n">
         <v>8.630000000000001</v>
       </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>3 ans</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>-3.98%</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>11.94</v>
+      </c>
+      <c r="H8" t="n">
+        <v>8.630000000000001</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -582,6 +698,22 @@
       <c r="D9" t="n">
         <v>8.630000000000001</v>
       </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>5 ans</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>-28.00%</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>15.38</v>
+      </c>
+      <c r="H9" t="n">
+        <v>8.630000000000001</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -600,6 +732,22 @@
       <c r="D10" t="n">
         <v>7.19</v>
       </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>10 ans</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>+41.76%</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>16.98</v>
+      </c>
+      <c r="H10" t="n">
+        <v>7.19</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -607,15 +755,23 @@
           <t>MM20</t>
         </is>
       </c>
-      <c r="B11" t="n">
-        <v/>
-      </c>
-      <c r="C11" t="n">
-        <v/>
-      </c>
       <c r="D11" t="n">
         <v>10.47</v>
       </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>MM20</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v/>
+      </c>
+      <c r="G11" t="n">
+        <v/>
+      </c>
+      <c r="H11" t="n">
+        <v>10.47</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -623,15 +779,23 @@
           <t>MM50</t>
         </is>
       </c>
-      <c r="B12" t="n">
-        <v/>
-      </c>
-      <c r="C12" t="n">
-        <v/>
-      </c>
       <c r="D12" t="n">
         <v>10.84</v>
       </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>MM50</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v/>
+      </c>
+      <c r="G12" t="n">
+        <v/>
+      </c>
+      <c r="H12" t="n">
+        <v>10.84</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -639,15 +803,23 @@
           <t>MM100</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v/>
-      </c>
-      <c r="C13" t="n">
-        <v/>
-      </c>
       <c r="D13" t="n">
         <v>10.98</v>
       </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>MM100</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v/>
+      </c>
+      <c r="G13" t="n">
+        <v/>
+      </c>
+      <c r="H13" t="n">
+        <v>10.98</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -655,20 +827,29 @@
           <t>RSI14</t>
         </is>
       </c>
-      <c r="B14" t="n">
-        <v/>
-      </c>
-      <c r="C14" t="n">
-        <v/>
-      </c>
       <c r="D14" t="n">
         <v>55.17</v>
       </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>RSI14</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v/>
+      </c>
+      <c r="G14" t="n">
+        <v/>
+      </c>
+      <c r="H14" t="n">
+        <v>55.17</v>
+      </c>
     </row>
     <row r="15"/>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:H1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -694,6 +875,11 @@
           <t>16-07-2023</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>16-07-2023</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -712,7 +898,22 @@
       <c r="D2" s="2" t="n">
         <v>20.69</v>
       </c>
-      <c r="E2" s="2" t="n"/>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>1er Janvier</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>+18.62%</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>28.41</v>
+      </c>
+      <c r="H2" t="n">
+        <v>20.69</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -731,6 +932,22 @@
       <c r="D3" t="n">
         <v>25.04</v>
       </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>1 semaine</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>+5.58%</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>27.24</v>
+      </c>
+      <c r="H3" t="n">
+        <v>25.04</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -749,6 +966,22 @@
       <c r="D4" t="n">
         <v>24.65</v>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>1 mois</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>+2.34%</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>27.81</v>
+      </c>
+      <c r="H4" t="n">
+        <v>24.65</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -767,6 +1000,22 @@
       <c r="D5" t="n">
         <v>21.43</v>
       </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>3 mois</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>+22.99%</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>28.07</v>
+      </c>
+      <c r="H5" t="n">
+        <v>21.43</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -785,6 +1034,22 @@
       <c r="D6" t="n">
         <v>20.69</v>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>6 mois</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>+4.32%</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>28.41</v>
+      </c>
+      <c r="H6" t="n">
+        <v>20.69</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -803,6 +1068,22 @@
       <c r="D7" t="n">
         <v>16.04</v>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>1 an</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>+13.74%</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>28.41</v>
+      </c>
+      <c r="H7" t="n">
+        <v>16.04</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -821,6 +1102,22 @@
       <c r="D8" t="n">
         <v>16.04</v>
       </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>3 ans</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>-37.87%</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>49.34</v>
+      </c>
+      <c r="H8" t="n">
+        <v>16.04</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -839,6 +1136,22 @@
       <c r="D9" t="n">
         <v>16.04</v>
       </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>5 ans</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>-23.37%</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>49.34</v>
+      </c>
+      <c r="H9" t="n">
+        <v>16.04</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -857,6 +1170,22 @@
       <c r="D10" t="n">
         <v>16.04</v>
       </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>10 ans</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>+18.78%</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>49.34</v>
+      </c>
+      <c r="H10" t="n">
+        <v>16.04</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -864,15 +1193,23 @@
           <t>MM20</t>
         </is>
       </c>
-      <c r="B11" t="n">
-        <v/>
-      </c>
-      <c r="C11" t="n">
-        <v/>
-      </c>
       <c r="D11" t="n">
         <v>26.57</v>
       </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>MM20</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v/>
+      </c>
+      <c r="G11" t="n">
+        <v/>
+      </c>
+      <c r="H11" t="n">
+        <v>26.57</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -880,15 +1217,23 @@
           <t>MM50</t>
         </is>
       </c>
-      <c r="B12" t="n">
-        <v/>
-      </c>
-      <c r="C12" t="n">
-        <v/>
-      </c>
       <c r="D12" t="n">
         <v>26.46</v>
       </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>MM50</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v/>
+      </c>
+      <c r="G12" t="n">
+        <v/>
+      </c>
+      <c r="H12" t="n">
+        <v>26.46</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -896,15 +1241,23 @@
           <t>MM100</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v/>
-      </c>
-      <c r="C13" t="n">
-        <v/>
-      </c>
       <c r="D13" t="n">
         <v>25.46</v>
       </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>MM100</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v/>
+      </c>
+      <c r="G13" t="n">
+        <v/>
+      </c>
+      <c r="H13" t="n">
+        <v>25.46</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -912,20 +1265,29 @@
           <t>RSI14</t>
         </is>
       </c>
-      <c r="B14" t="n">
-        <v/>
-      </c>
-      <c r="C14" t="n">
-        <v/>
-      </c>
       <c r="D14" t="n">
         <v>45.39</v>
       </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>RSI14</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v/>
+      </c>
+      <c r="G14" t="n">
+        <v/>
+      </c>
+      <c r="H14" t="n">
+        <v>45.39</v>
+      </c>
     </row>
     <row r="15"/>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:H1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>